<commit_message>
Restore essential OCR and agent modules, rerun pipeline with real PDF, update outputs.
</commit_message>
<xml_diff>
--- a/balance_rag.xlsx
+++ b/balance_rag.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
   <si>
     <t>Cuenta</t>
   </si>
@@ -25,15 +25,15 @@
     <t>Valor</t>
   </si>
   <si>
-    <t>cuentas comerciales por cobrar y otras cuentas por cobrar corrientes</t>
-  </si>
-  <si>
     <t>cuentas comerciales por cobrar y otras cuentas por cobrar no corrientes</t>
   </si>
   <si>
     <t>inversiones contabilizadas utilizando el método de la participación</t>
   </si>
   <si>
+    <t>Inversiones contabilizadas utilizando el método de la participación</t>
+  </si>
+  <si>
     <t>Activos intangibles distintos de la plusvalía</t>
   </si>
   <si>
@@ -52,241 +52,244 @@
     <t>efectivo y equivalentes</t>
   </si>
   <si>
-    <t>875461204</t>
-  </si>
-  <si>
     <t>138313</t>
   </si>
   <si>
     <t>331502901</t>
   </si>
   <si>
+    <t>334657003</t>
+  </si>
+  <si>
     <t>774003943</t>
   </si>
   <si>
     <t>1873590001</t>
   </si>
   <si>
+    <t>4110735696</t>
+  </si>
+  <si>
+    <t>3392498650</t>
+  </si>
+  <si>
+    <t>369637458</t>
+  </si>
+  <si>
+    <t>378697266</t>
+  </si>
+  <si>
+    <t>Cuentas por pagar comerciales y otras cuentas por pagar</t>
+  </si>
+  <si>
+    <t>Provisiones corrientes por beneficios a los empleados</t>
+  </si>
+  <si>
+    <t>cuentas comerciales por pagar y otras cuentas por pagar no corrientes</t>
+  </si>
+  <si>
+    <t>Provisiones no corrientes por beneficios a los empleados</t>
+  </si>
+  <si>
+    <t>2653580482</t>
+  </si>
+  <si>
+    <t>136878132</t>
+  </si>
+  <si>
+    <t>3401565</t>
+  </si>
+  <si>
+    <t>3263065</t>
+  </si>
+  <si>
+    <t>capital</t>
+  </si>
+  <si>
+    <t>utilidades retenidas</t>
+  </si>
+  <si>
+    <t>prima de emisión</t>
+  </si>
+  <si>
+    <t>otras reservas</t>
+  </si>
+  <si>
+    <t>participaciones no controladoras</t>
+  </si>
+  <si>
+    <t>Participaciones no controladoras</t>
+  </si>
+  <si>
+    <t>atribuible a participaciones no controladoras</t>
+  </si>
+  <si>
+    <t>2380288909</t>
+  </si>
+  <si>
+    <t>2078932098</t>
+  </si>
+  <si>
+    <t>459360260</t>
+  </si>
+  <si>
+    <t>633715769</t>
+  </si>
+  <si>
+    <t>607015945</t>
+  </si>
+  <si>
+    <t>15513358</t>
+  </si>
+  <si>
+    <t>MS ACTIVOS CORRIENTES Efectivo y equivalentes al efectivo</t>
+  </si>
+  <si>
+    <t>Otros activos financieros corrientes</t>
+  </si>
+  <si>
+    <t>Otros activos no financieros corrientes</t>
+  </si>
+  <si>
+    <t>Cuentas comerciales por cobrar y otras cuentas por cobrar corrientes</t>
+  </si>
+  <si>
+    <t>corrientes</t>
+  </si>
+  <si>
+    <t>Inventarios corrientes</t>
+  </si>
+  <si>
+    <t>ACTIVOS NO CORRIENTES Otros activos financieros no corrientes</t>
+  </si>
+  <si>
+    <t>Otros activos no financieros no corrientes</t>
+  </si>
+  <si>
+    <t>Cuentas comerciales por cobrar y otras cuentas por cobrar no corrientes</t>
+  </si>
+  <si>
+    <t>Plusvalía</t>
+  </si>
+  <si>
+    <t>no corrientes</t>
+  </si>
+  <si>
+    <t>MS PASIVOS CORRIENTES Otros pasivos financieros corrientes</t>
+  </si>
+  <si>
+    <t>Otras provisiones corrientes</t>
+  </si>
+  <si>
+    <t>Otros pasivos no financieros corrientes</t>
+  </si>
+  <si>
+    <t>PASIVOS NO CORRIENTES Otros pasivos financieros no corrientes</t>
+  </si>
+  <si>
+    <t>Pasivos por arrendamientos no corrientes</t>
+  </si>
+  <si>
+    <t>Cuentas comerciales por pagar y otras cuentas por pagar no corrientes</t>
+  </si>
+  <si>
+    <t>Otras provisiones no corrientes</t>
+  </si>
+  <si>
+    <t>Pasivo por impuestos diferidos</t>
+  </si>
+  <si>
+    <t>Otros pasivos no financieros no corrientes</t>
+  </si>
+  <si>
+    <t>MS MS Ingresos de actividades ordinarias</t>
+  </si>
+  <si>
+    <t>Otros ingresos</t>
+  </si>
+  <si>
+    <t>Ingresos financieros</t>
+  </si>
+  <si>
+    <t>Efectivo y equivalentes al efectivo al principio del período</t>
+  </si>
+  <si>
+    <t>Efectivo y equivalentes al efectivo al final del período</t>
+  </si>
+  <si>
+    <t>483125584</t>
+  </si>
+  <si>
+    <t>211081454</t>
+  </si>
+  <si>
+    <t>32698910</t>
+  </si>
+  <si>
+    <t>701683203</t>
+  </si>
+  <si>
+    <t>48325022</t>
+  </si>
+  <si>
+    <t>1411220909</t>
+  </si>
+  <si>
+    <t>230585174</t>
+  </si>
+  <si>
+    <t>26479028</t>
+  </si>
+  <si>
+    <t>156599</t>
+  </si>
+  <si>
+    <t>862236570</t>
+  </si>
+  <si>
+    <t>2059796230</t>
+  </si>
+  <si>
     <t>3743122719</t>
   </si>
   <si>
     <t>3188927576</t>
   </si>
   <si>
+    <t>4046018</t>
+  </si>
+  <si>
     <t>356550480</t>
   </si>
   <si>
-    <t>378697266</t>
-  </si>
-  <si>
-    <t>Cuentas por pagar comerciales y otras cuentas por pagar</t>
-  </si>
-  <si>
-    <t>Provisiones corrientes por beneficios a los empleados</t>
-  </si>
-  <si>
-    <t>cuentas comerciales por pagar y otras cuentas por pagar no corrientes</t>
-  </si>
-  <si>
-    <t>Provisiones no corrientes por beneficios a los empleados</t>
+    <t>505461062</t>
   </si>
   <si>
     <t>2866975457</t>
   </si>
   <si>
-    <t>136878132</t>
+    <t>16826672</t>
+  </si>
+  <si>
+    <t>130178251</t>
+  </si>
+  <si>
+    <t>240505744</t>
+  </si>
+  <si>
+    <t>3704831700</t>
+  </si>
+  <si>
+    <t>1098575638</t>
   </si>
   <si>
     <t>3536289</t>
   </si>
   <si>
-    <t>5435730</t>
-  </si>
-  <si>
-    <t>capital</t>
-  </si>
-  <si>
-    <t>utilidades retenidas</t>
-  </si>
-  <si>
-    <t>prima de emisión</t>
-  </si>
-  <si>
-    <t>Prima de emisión</t>
-  </si>
-  <si>
-    <t>participaciones no controladoras</t>
-  </si>
-  <si>
-    <t>atribuciones no controladoras</t>
-  </si>
-  <si>
-    <t>atribuible a participaciones no controladoras</t>
-  </si>
-  <si>
-    <t>2380288909</t>
-  </si>
-  <si>
-    <t>2078932098</t>
-  </si>
-  <si>
-    <t>459360260</t>
-  </si>
-  <si>
-    <t>607015945</t>
-  </si>
-  <si>
-    <t>22019318</t>
-  </si>
-  <si>
-    <t>15513358</t>
-  </si>
-  <si>
-    <t>MS ACTIVOS CORRIENTES Efectivo y equivalentes al efectivo</t>
-  </si>
-  <si>
-    <t>Otros activos financieros corrientes</t>
-  </si>
-  <si>
-    <t>Otros activos no financieros corrientes</t>
-  </si>
-  <si>
-    <t>Cuentas comerciales por cobrar y otras cuentas por cobrar corrientes</t>
-  </si>
-  <si>
-    <t>corrientes</t>
-  </si>
-  <si>
-    <t>Inventarios corrientes</t>
-  </si>
-  <si>
-    <t>ACTIVOS NO CORRIENTES Otros activos financieros no corrientes</t>
-  </si>
-  <si>
-    <t>Otros activos no financieros no corrientes</t>
-  </si>
-  <si>
-    <t>Cuentas comerciales por cobrar y otras cuentas por cobrar no corrientes</t>
-  </si>
-  <si>
-    <t>Inversiones contabilizadas utilizando el método de la participación</t>
-  </si>
-  <si>
-    <t>no corrientes</t>
-  </si>
-  <si>
-    <t>MS PASIVOS CORRIENTES Otros pasivos financieros corrientes</t>
-  </si>
-  <si>
-    <t>Otras provisiones corrientes</t>
-  </si>
-  <si>
-    <t>Otros pasivos no financieros corrientes</t>
-  </si>
-  <si>
-    <t>PASIVOS NO CORRIENTES Otros pasivos financieros no corrientes</t>
-  </si>
-  <si>
-    <t>Pasivos por arrendamientos no corrientes</t>
-  </si>
-  <si>
-    <t>Cuentas comerciales por pagar y otras cuentas por pagar no corrientes</t>
-  </si>
-  <si>
-    <t>Otras provisiones no corrientes</t>
-  </si>
-  <si>
-    <t>Pasivo por impuestos diferidos</t>
-  </si>
-  <si>
-    <t>Otros pasivos no financieros no corrientes</t>
-  </si>
-  <si>
-    <t>MS MS Ingresos de actividades ordinarias</t>
-  </si>
-  <si>
-    <t>Otros ingresos</t>
-  </si>
-  <si>
-    <t>Ingresos financieros</t>
-  </si>
-  <si>
-    <t>Efectivo y equivalentes al efectivo al principio del período</t>
-  </si>
-  <si>
-    <t>Efectivo y equivalentes al efectivo al final del período</t>
-  </si>
-  <si>
-    <t>483125584</t>
-  </si>
-  <si>
-    <t>211081454</t>
-  </si>
-  <si>
-    <t>32698910</t>
-  </si>
-  <si>
-    <t>701683203</t>
-  </si>
-  <si>
-    <t>48325022</t>
-  </si>
-  <si>
-    <t>1411220909</t>
-  </si>
-  <si>
-    <t>230585174</t>
-  </si>
-  <si>
-    <t>26479028</t>
-  </si>
-  <si>
-    <t>156599</t>
-  </si>
-  <si>
-    <t>334657003</t>
-  </si>
-  <si>
-    <t>862236570</t>
-  </si>
-  <si>
-    <t>3392498650</t>
-  </si>
-  <si>
-    <t>4046018</t>
-  </si>
-  <si>
-    <t>505461062</t>
-  </si>
-  <si>
-    <t>2653580482</t>
-  </si>
-  <si>
-    <t>16826672</t>
-  </si>
-  <si>
-    <t>130178251</t>
-  </si>
-  <si>
-    <t>240505744</t>
-  </si>
-  <si>
-    <t>3704831700</t>
-  </si>
-  <si>
-    <t>1098575638</t>
-  </si>
-  <si>
-    <t>3401565</t>
-  </si>
-  <si>
     <t>48070186</t>
   </si>
   <si>
     <t>558350832</t>
-  </si>
-  <si>
-    <t>3263065</t>
   </si>
   <si>
     <t>76027357</t>
@@ -885,7 +888,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -973,7 +976,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>75</v>
@@ -981,7 +984,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
         <v>76</v>
@@ -989,7 +992,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>77</v>
@@ -997,7 +1000,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
         <v>78</v>
@@ -1005,7 +1008,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
         <v>79</v>
@@ -1013,7 +1016,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
         <v>80</v>
@@ -1021,7 +1024,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
         <v>81</v>
@@ -1029,7 +1032,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
         <v>82</v>
@@ -1037,7 +1040,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
         <v>83</v>
@@ -1045,7 +1048,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>84</v>
@@ -1053,7 +1056,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
         <v>85</v>
@@ -1061,7 +1064,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
         <v>86</v>
@@ -1069,7 +1072,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
         <v>87</v>
@@ -1077,7 +1080,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
         <v>88</v>
@@ -1085,7 +1088,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
         <v>89</v>
@@ -1093,7 +1096,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
         <v>90</v>
@@ -1101,7 +1104,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
         <v>91</v>
@@ -1109,7 +1112,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
         <v>92</v>
@@ -1117,7 +1120,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
         <v>93</v>
@@ -1125,7 +1128,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
         <v>94</v>
@@ -1133,10 +1136,18 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run pipeline with real PDF from document/, update extracted_terms.csv and balance_rag.xlsx with new results.
</commit_message>
<xml_diff>
--- a/balance_rag.xlsx
+++ b/balance_rag.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
   <si>
     <t>Cuenta</t>
   </si>
@@ -25,289 +25,268 @@
     <t>Valor</t>
   </si>
   <si>
-    <t>cuentas comerciales por cobrar y otras cuentas por cobrar no corrientes</t>
-  </si>
-  <si>
     <t>inversiones contabilizadas utilizando el método de la participación</t>
   </si>
   <si>
+    <t>Activos intangibles distintos de la plusvalía</t>
+  </si>
+  <si>
+    <t>plusvalía</t>
+  </si>
+  <si>
+    <t>Plusvalía</t>
+  </si>
+  <si>
+    <t>planta y equipo</t>
+  </si>
+  <si>
+    <t>Propiedad de inversión</t>
+  </si>
+  <si>
+    <t>Activos por impuestos diferidos</t>
+  </si>
+  <si>
+    <t>efectivo y equivalentes</t>
+  </si>
+  <si>
+    <t>331502901</t>
+  </si>
+  <si>
+    <t>774003943</t>
+  </si>
+  <si>
+    <t>2059796230</t>
+  </si>
+  <si>
+    <t>1873590001</t>
+  </si>
+  <si>
+    <t>3743122719</t>
+  </si>
+  <si>
+    <t>3188927576</t>
+  </si>
+  <si>
+    <t>356550480</t>
+  </si>
+  <si>
+    <t>378697266</t>
+  </si>
+  <si>
+    <t>cuentas por pagar comerciales y otras cuentas por pagar</t>
+  </si>
+  <si>
+    <t>Provisiones no corrientes por beneficios a los empleados</t>
+  </si>
+  <si>
+    <t>2866975457</t>
+  </si>
+  <si>
+    <t>5435730</t>
+  </si>
+  <si>
+    <t>capital</t>
+  </si>
+  <si>
+    <t>utilidades retenidas</t>
+  </si>
+  <si>
+    <t>prima de emisión</t>
+  </si>
+  <si>
+    <t>otras reservas</t>
+  </si>
+  <si>
+    <t>Participaciones no controladoras</t>
+  </si>
+  <si>
+    <t>resultado del ejercicio</t>
+  </si>
+  <si>
+    <t>atribuible a participaciones no controladoras</t>
+  </si>
+  <si>
+    <t>2380288909</t>
+  </si>
+  <si>
+    <t>2078932098</t>
+  </si>
+  <si>
+    <t>459360260</t>
+  </si>
+  <si>
+    <t>607015945</t>
+  </si>
+  <si>
+    <t>3503183757</t>
+  </si>
+  <si>
+    <t>22019318</t>
+  </si>
+  <si>
+    <t>MS ACTIVOS CORRIENTES Efectivo y equivalentes al efectivo</t>
+  </si>
+  <si>
+    <t>Otros activos financieros corrientes</t>
+  </si>
+  <si>
+    <t>Otros activos no financieros corrientes</t>
+  </si>
+  <si>
+    <t>Cuentas comerciales por cobrar y otras cuentas por cobrar corrientes</t>
+  </si>
+  <si>
+    <t>corrientes</t>
+  </si>
+  <si>
+    <t>Inventarios corrientes</t>
+  </si>
+  <si>
+    <t>ACTIVOS NO CORRIENTES Otros activos financieros no corrientes</t>
+  </si>
+  <si>
+    <t>Otros activos no financieros no corrientes</t>
+  </si>
+  <si>
+    <t>Cuentas comerciales por cobrar y otras cuentas por cobrar no corrientes</t>
+  </si>
+  <si>
     <t>Inversiones contabilizadas utilizando el método de la participación</t>
   </si>
   <si>
-    <t>Activos intangibles distintos de la plusvalía</t>
-  </si>
-  <si>
-    <t>plusvalía</t>
-  </si>
-  <si>
-    <t>planta y equipo</t>
-  </si>
-  <si>
-    <t>Propiedad de inversión</t>
-  </si>
-  <si>
-    <t>Activos por impuestos diferidos</t>
-  </si>
-  <si>
-    <t>efectivo y equivalentes</t>
-  </si>
-  <si>
-    <t>138313</t>
-  </si>
-  <si>
-    <t>331502901</t>
+    <t>no corrientes</t>
+  </si>
+  <si>
+    <t>MS PASIVOS CORRIENTES Otros pasivos financieros corrientes</t>
+  </si>
+  <si>
+    <t>Cuentas por pagar comerciales y otras cuentas por pagar</t>
+  </si>
+  <si>
+    <t>Otras provisiones corrientes</t>
+  </si>
+  <si>
+    <t>Provisiones corrientes por beneficios a los empleados</t>
+  </si>
+  <si>
+    <t>Otros pasivos no financieros corrientes</t>
+  </si>
+  <si>
+    <t>PASIVOS NO CORRIENTES Otros pasivos financieros no corrientes</t>
+  </si>
+  <si>
+    <t>Pasivos por arrendamientos no corrientes</t>
+  </si>
+  <si>
+    <t>Cuentas comerciales por pagar y otras cuentas por pagar no corrientes</t>
+  </si>
+  <si>
+    <t>Otras provisiones no corrientes</t>
+  </si>
+  <si>
+    <t>Pasivo por impuestos diferidos</t>
+  </si>
+  <si>
+    <t>Otros pasivos no financieros no corrientes</t>
+  </si>
+  <si>
+    <t>MS MS Ingresos de actividades ordinarias</t>
+  </si>
+  <si>
+    <t>Otros ingresos</t>
+  </si>
+  <si>
+    <t>Ingresos financieros</t>
+  </si>
+  <si>
+    <t>Efectivo y equivalentes al efectivo al principio del período</t>
+  </si>
+  <si>
+    <t>483125584</t>
+  </si>
+  <si>
+    <t>211081454</t>
+  </si>
+  <si>
+    <t>32698910</t>
+  </si>
+  <si>
+    <t>701683203</t>
+  </si>
+  <si>
+    <t>48325022</t>
+  </si>
+  <si>
+    <t>1411220909</t>
+  </si>
+  <si>
+    <t>230585174</t>
+  </si>
+  <si>
+    <t>26479028</t>
+  </si>
+  <si>
+    <t>156599</t>
   </si>
   <si>
     <t>334657003</t>
   </si>
   <si>
-    <t>774003943</t>
-  </si>
-  <si>
-    <t>1873590001</t>
-  </si>
-  <si>
     <t>4110735696</t>
   </si>
   <si>
-    <t>3392498650</t>
-  </si>
-  <si>
-    <t>369637458</t>
-  </si>
-  <si>
-    <t>378697266</t>
-  </si>
-  <si>
-    <t>Cuentas por pagar comerciales y otras cuentas por pagar</t>
-  </si>
-  <si>
-    <t>Provisiones corrientes por beneficios a los empleados</t>
-  </si>
-  <si>
-    <t>cuentas comerciales por pagar y otras cuentas por pagar no corrientes</t>
-  </si>
-  <si>
-    <t>Provisiones no corrientes por beneficios a los empleados</t>
+    <t>4046018</t>
+  </si>
+  <si>
+    <t>505461062</t>
   </si>
   <si>
     <t>2653580482</t>
   </si>
   <si>
+    <t>16826672</t>
+  </si>
+  <si>
     <t>136878132</t>
   </si>
   <si>
+    <t>240505744</t>
+  </si>
+  <si>
+    <t>3704831700</t>
+  </si>
+  <si>
+    <t>1098575638</t>
+  </si>
+  <si>
     <t>3401565</t>
   </si>
   <si>
+    <t>48070186</t>
+  </si>
+  <si>
+    <t>558350832</t>
+  </si>
+  <si>
     <t>3263065</t>
   </si>
   <si>
-    <t>capital</t>
-  </si>
-  <si>
-    <t>utilidades retenidas</t>
-  </si>
-  <si>
-    <t>prima de emisión</t>
-  </si>
-  <si>
-    <t>otras reservas</t>
-  </si>
-  <si>
-    <t>participaciones no controladoras</t>
-  </si>
-  <si>
-    <t>Participaciones no controladoras</t>
-  </si>
-  <si>
-    <t>atribuible a participaciones no controladoras</t>
-  </si>
-  <si>
-    <t>2380288909</t>
-  </si>
-  <si>
-    <t>2078932098</t>
-  </si>
-  <si>
-    <t>459360260</t>
-  </si>
-  <si>
-    <t>633715769</t>
-  </si>
-  <si>
-    <t>607015945</t>
+    <t>76027357</t>
+  </si>
+  <si>
+    <t>3938069983</t>
+  </si>
+  <si>
+    <t>8518912</t>
+  </si>
+  <si>
+    <t>4602195</t>
   </si>
   <si>
     <t>15513358</t>
   </si>
   <si>
-    <t>MS ACTIVOS CORRIENTES Efectivo y equivalentes al efectivo</t>
-  </si>
-  <si>
-    <t>Otros activos financieros corrientes</t>
-  </si>
-  <si>
-    <t>Otros activos no financieros corrientes</t>
-  </si>
-  <si>
-    <t>Cuentas comerciales por cobrar y otras cuentas por cobrar corrientes</t>
-  </si>
-  <si>
-    <t>corrientes</t>
-  </si>
-  <si>
-    <t>Inventarios corrientes</t>
-  </si>
-  <si>
-    <t>ACTIVOS NO CORRIENTES Otros activos financieros no corrientes</t>
-  </si>
-  <si>
-    <t>Otros activos no financieros no corrientes</t>
-  </si>
-  <si>
-    <t>Cuentas comerciales por cobrar y otras cuentas por cobrar no corrientes</t>
-  </si>
-  <si>
-    <t>Plusvalía</t>
-  </si>
-  <si>
-    <t>no corrientes</t>
-  </si>
-  <si>
-    <t>MS PASIVOS CORRIENTES Otros pasivos financieros corrientes</t>
-  </si>
-  <si>
-    <t>Otras provisiones corrientes</t>
-  </si>
-  <si>
-    <t>Otros pasivos no financieros corrientes</t>
-  </si>
-  <si>
-    <t>PASIVOS NO CORRIENTES Otros pasivos financieros no corrientes</t>
-  </si>
-  <si>
-    <t>Pasivos por arrendamientos no corrientes</t>
-  </si>
-  <si>
-    <t>Cuentas comerciales por pagar y otras cuentas por pagar no corrientes</t>
-  </si>
-  <si>
-    <t>Otras provisiones no corrientes</t>
-  </si>
-  <si>
-    <t>Pasivo por impuestos diferidos</t>
-  </si>
-  <si>
-    <t>Otros pasivos no financieros no corrientes</t>
-  </si>
-  <si>
-    <t>MS MS Ingresos de actividades ordinarias</t>
-  </si>
-  <si>
-    <t>Otros ingresos</t>
-  </si>
-  <si>
-    <t>Ingresos financieros</t>
-  </si>
-  <si>
-    <t>Efectivo y equivalentes al efectivo al principio del período</t>
-  </si>
-  <si>
-    <t>Efectivo y equivalentes al efectivo al final del período</t>
-  </si>
-  <si>
-    <t>483125584</t>
-  </si>
-  <si>
-    <t>211081454</t>
-  </si>
-  <si>
-    <t>32698910</t>
-  </si>
-  <si>
-    <t>701683203</t>
-  </si>
-  <si>
-    <t>48325022</t>
-  </si>
-  <si>
-    <t>1411220909</t>
-  </si>
-  <si>
-    <t>230585174</t>
-  </si>
-  <si>
-    <t>26479028</t>
-  </si>
-  <si>
-    <t>156599</t>
-  </si>
-  <si>
-    <t>862236570</t>
-  </si>
-  <si>
-    <t>2059796230</t>
-  </si>
-  <si>
-    <t>3743122719</t>
-  </si>
-  <si>
-    <t>3188927576</t>
-  </si>
-  <si>
-    <t>4046018</t>
-  </si>
-  <si>
-    <t>356550480</t>
-  </si>
-  <si>
-    <t>505461062</t>
-  </si>
-  <si>
-    <t>2866975457</t>
-  </si>
-  <si>
-    <t>16826672</t>
-  </si>
-  <si>
-    <t>130178251</t>
-  </si>
-  <si>
-    <t>240505744</t>
-  </si>
-  <si>
-    <t>3704831700</t>
-  </si>
-  <si>
-    <t>1098575638</t>
-  </si>
-  <si>
-    <t>3536289</t>
-  </si>
-  <si>
-    <t>48070186</t>
-  </si>
-  <si>
-    <t>558350832</t>
-  </si>
-  <si>
-    <t>76027357</t>
-  </si>
-  <si>
-    <t>3503183757</t>
-  </si>
-  <si>
-    <t>8518912</t>
-  </si>
-  <si>
-    <t>4602195</t>
-  </si>
-  <si>
     <t>373700303</t>
-  </si>
-  <si>
-    <t>564926038</t>
   </si>
 </sst>
 </file>
@@ -665,7 +644,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -684,7 +663,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -692,7 +671,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -700,7 +679,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -708,7 +687,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -716,7 +695,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -724,7 +703,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -732,7 +711,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -740,15 +719,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -758,7 +729,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -774,34 +745,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -827,58 +782,58 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
         <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -888,7 +843,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -904,250 +859,234 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>